<commit_message>
Final results :)). Need to write discussion, conclusion and abstract
</commit_message>
<xml_diff>
--- a/results/hyperparemeter_search.xlsx
+++ b/results/hyperparemeter_search.xlsx
@@ -2463,8 +2463,8 @@
   </sheetPr>
   <dimension ref="A1:K847"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A825" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A725" activeCellId="0" sqref="A725"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A832" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D847" activeCellId="0" sqref="D847"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -18198,6 +18198,9 @@
       </c>
       <c r="D845" s="0" t="n">
         <v>23</v>
+      </c>
+      <c r="E845" s="0" t="n">
+        <v>0.207</v>
       </c>
       <c r="F845" s="0" t="s">
         <v>287</v>

</xml_diff>